<commit_message>
feat(pipelining): add testing program for register data processing instruction which is followed by LDST that needs to access the register file #23
</commit_message>
<xml_diff>
--- a/programs/loadinstructionsnohazard.xlsx
+++ b/programs/loadinstructionsnohazard.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vacla\Projects\cpu\programs\pipelining\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vacla\Projects\cpu\programs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D2ABD5B-1A87-47DA-9FDF-BAF0BA65E93F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C2221EA-69AA-4C37-956B-7794498A72FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{E410B2C1-F054-41C4-A96D-F1120FBD95E0}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{E410B2C1-F054-41C4-A96D-F1120FBD95E0}"/>
   </bookViews>
   <sheets>
     <sheet name="Code" sheetId="1" r:id="rId1"/>
@@ -246,10 +246,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -632,33 +632,33 @@
       <c r="C2" s="1">
         <v>1</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6" t="s">
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="6"/>
+      <c r="H2" s="7"/>
       <c r="I2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="K2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6" t="s">
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="O2" s="6"/>
-      <c r="P2" s="6"/>
-      <c r="Q2" s="6"/>
-      <c r="R2" s="6"/>
+      <c r="O2" s="7"/>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="7"/>
+      <c r="R2" s="7"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
@@ -667,35 +667,35 @@
       <c r="C3" s="1">
         <v>1</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6" t="s">
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="6"/>
+      <c r="H3" s="7"/>
       <c r="I3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="K3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
-      <c r="O3" s="6" t="s">
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="P3" s="6"/>
-      <c r="Q3" s="6" t="s">
+      <c r="P3" s="7"/>
+      <c r="Q3" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="R3" s="6"/>
+      <c r="R3" s="7"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
@@ -713,10 +713,10 @@
       <c r="F4" s="1">
         <v>0</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="6"/>
+      <c r="H4" s="7"/>
       <c r="I4" s="1" t="s">
         <v>14</v>
       </c>
@@ -729,16 +729,16 @@
       <c r="L4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="6" t="s">
+      <c r="M4" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="N4" s="6"/>
-      <c r="O4" s="6"/>
-      <c r="P4" s="6"/>
-      <c r="Q4" s="6" t="s">
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
+      <c r="P4" s="7"/>
+      <c r="Q4" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="R4" s="6"/>
+      <c r="R4" s="7"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
@@ -747,56 +747,56 @@
       <c r="C5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6" t="s">
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
-      <c r="N5" s="6"/>
-      <c r="O5" s="6"/>
-      <c r="P5" s="6"/>
-      <c r="Q5" s="6"/>
-      <c r="R5" s="6"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="7"/>
+      <c r="P5" s="7"/>
+      <c r="Q5" s="7"/>
+      <c r="R5" s="7"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6" t="s">
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6" t="s">
+      <c r="H6" s="7"/>
+      <c r="I6" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6" t="s">
+      <c r="J6" s="7"/>
+      <c r="K6" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="L6" s="6"/>
-      <c r="M6" s="6"/>
-      <c r="N6" s="6"/>
-      <c r="O6" s="6"/>
-      <c r="P6" s="6"/>
-      <c r="Q6" s="6" t="s">
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="7"/>
+      <c r="O6" s="7"/>
+      <c r="P6" s="7"/>
+      <c r="Q6" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="R6" s="6"/>
+      <c r="R6" s="7"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="C7" s="3"/>
@@ -1116,6 +1116,16 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="M4:P4"/>
+    <mergeCell ref="Q4:R4"/>
+    <mergeCell ref="D5:H5"/>
+    <mergeCell ref="I5:R5"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="Q6:R6"/>
+    <mergeCell ref="K6:P6"/>
     <mergeCell ref="D2:F2"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="K2:M2"/>
@@ -1125,16 +1135,6 @@
     <mergeCell ref="K3:N3"/>
     <mergeCell ref="O3:P3"/>
     <mergeCell ref="Q3:R3"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="Q6:R6"/>
-    <mergeCell ref="K6:P6"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="M4:P4"/>
-    <mergeCell ref="Q4:R4"/>
-    <mergeCell ref="D5:H5"/>
-    <mergeCell ref="I5:R5"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1147,7 +1147,7 @@
   <dimension ref="A1:O14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1157,30 +1157,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
       <c r="D2">
         <v>0</v>
       </c>
@@ -1285,21 +1285,21 @@
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
-      <c r="N8" s="7"/>
-      <c r="O8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D9">

</xml_diff>